<commit_message>
add excel download and set dark mode
</commit_message>
<xml_diff>
--- a/public/pdf/mycv.xlsx
+++ b/public/pdf/mycv.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="177">
   <si>
     <t>履歴書</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve"> 月</t>
   </si>
   <si>
-    <t>7</t>
+    <t>25</t>
   </si>
   <si>
     <t>日</t>
@@ -330,9 +330,6 @@
       </rPr>
       <t>居 住 地</t>
     </r>
-  </si>
-  <si>
-    <t>東京都</t>
   </si>
   <si>
     <r>
@@ -1360,9 +1357,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="6" formatCode="&quot;\&quot;#,##0;[Red]&quot;\&quot;\-#,##0"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_-&quot;\&quot;* #,##0_-\ ;\-&quot;\&quot;* #,##0_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
     <numFmt numFmtId="178" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
     <numFmt numFmtId="179" formatCode="&quot;&quot;#&quot;歳&quot;"/>
@@ -1479,11 +1476,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color indexed="12"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <charset val="128"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1494,7 +1491,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1502,14 +1499,37 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color indexed="12"/>
+      <name val="ＭＳ Ｐ明朝"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1562,46 +1582,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1616,15 +1598,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <name val="ＭＳ Ｐ明朝"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="ＭＳ Ｐ明朝"/>
-      <charset val="128"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1660,25 +1657,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1690,37 +1711,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1738,13 +1735,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1756,7 +1783,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1768,25 +1807,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1796,48 +1835,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="181">
     <border>
@@ -4041,6 +4038,84 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -4053,54 +4128,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -4111,36 +4138,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -4164,132 +4161,132 @@
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="174" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="175" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="175" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="176" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="176" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="177" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="176" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="174" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="173" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="178" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="173" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="179" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="180" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="175" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="177" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="179" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="19" borderId="180" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="19" borderId="179" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="173" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="178" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="0"/>
@@ -5754,7 +5751,7 @@
   <dimension ref="A1:AS55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScalePageLayoutView="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="AZ11" sqref="AZ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -7941,11 +7938,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC32:AE32">
+      <formula1>"[▼選択],正社員,役員,契約社員,派遣社員,嘱託・委託,アルバイト・パート,その他"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="配偶者の有無" prompt="選択してください" sqref="V6:Y6">
       <formula1>$AI$8:$AI$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC32:AE32">
-      <formula1>"[▼選択],正社員,役員,契約社員,派遣社員,嘱託・委託,アルバイト・パート,その他"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6:K7">
       <formula1>$AI$5:$AI$7</formula1>
@@ -7967,8 +7964,8 @@
   </sheetPr>
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="70" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="Z31" sqref="Z31"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.44166666666667" defaultRowHeight="19.5"/>
@@ -8062,12 +8059,12 @@
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="15"/>
       <c r="G5" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H5" s="17"/>
       <c r="I5" s="116">
@@ -8086,18 +8083,18 @@
     </row>
     <row r="6" ht="21" customHeight="1" spans="2:19">
       <c r="B6" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="18"/>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
       <c r="G6" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="118" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J6" s="119"/>
       <c r="K6" s="119"/>
@@ -8112,20 +8109,20 @@
     </row>
     <row r="7" ht="41.85" customHeight="1" spans="2:19">
       <c r="B7" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="24"/>
       <c r="F7" s="25"/>
       <c r="G7" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="120" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J7" s="121"/>
       <c r="K7" s="121"/>
@@ -8159,11 +8156,11 @@
     </row>
     <row r="9" ht="28.5" customHeight="1" spans="2:18">
       <c r="B9" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
@@ -8182,11 +8179,11 @@
     </row>
     <row r="10" ht="28.5" customHeight="1" spans="2:18">
       <c r="B10" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
@@ -8205,11 +8202,11 @@
     </row>
     <row r="11" ht="28.5" customHeight="1" spans="2:18">
       <c r="B11" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="35"/>
       <c r="D11" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" s="36"/>
       <c r="F11" s="36"/>
@@ -8247,31 +8244,31 @@
     </row>
     <row r="13" ht="19.35" customHeight="1" spans="2:18">
       <c r="B13" s="38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
       <c r="E13" s="39"/>
       <c r="F13" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="H13" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="H13" s="41" t="s">
+      <c r="I13" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="I13" s="41" t="s">
+      <c r="J13" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="J13" s="41" t="s">
+      <c r="K13" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="K13" s="41" t="s">
+      <c r="L13" s="122" t="s">
         <v>109</v>
-      </c>
-      <c r="L13" s="122" t="s">
-        <v>110</v>
       </c>
       <c r="M13" s="122"/>
       <c r="N13" s="122"/>
@@ -8292,25 +8289,25 @@
       <c r="J14" s="45"/>
       <c r="K14" s="45"/>
       <c r="L14" s="123" t="s">
+        <v>110</v>
+      </c>
+      <c r="M14" s="123" t="s">
         <v>111</v>
       </c>
-      <c r="M14" s="123" t="s">
+      <c r="N14" s="123" t="s">
         <v>112</v>
       </c>
-      <c r="N14" s="123" t="s">
+      <c r="O14" s="123" t="s">
         <v>113</v>
       </c>
-      <c r="O14" s="123" t="s">
+      <c r="P14" s="123" t="s">
         <v>114</v>
       </c>
-      <c r="P14" s="123" t="s">
+      <c r="Q14" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="Q14" s="123" t="s">
+      <c r="R14" s="151" t="s">
         <v>116</v>
-      </c>
-      <c r="R14" s="151" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="15" customFormat="1" ht="23.25" customHeight="1" spans="1:23">
@@ -8319,43 +8316,43 @@
         <v>1</v>
       </c>
       <c r="C15" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="E15" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="E15" s="49" t="s">
+      <c r="F15" s="50" t="s">
         <v>120</v>
-      </c>
-      <c r="F15" s="50" t="s">
-        <v>121</v>
       </c>
       <c r="G15" s="51"/>
       <c r="H15" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="I15" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="I15" s="52" t="s">
+      <c r="J15" s="124" t="s">
         <v>123</v>
       </c>
-      <c r="J15" s="124" t="s">
+      <c r="K15" s="52" t="s">
         <v>124</v>
-      </c>
-      <c r="K15" s="52" t="s">
-        <v>125</v>
       </c>
       <c r="L15" s="125"/>
       <c r="M15" s="125"/>
       <c r="N15" s="125" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O15" s="125" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P15" s="125" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q15" s="125" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="R15" s="152"/>
       <c r="S15" s="46"/>
@@ -8371,10 +8368,10 @@
       <c r="D16" s="55"/>
       <c r="E16" s="56"/>
       <c r="F16" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" s="58" t="s">
         <v>127</v>
-      </c>
-      <c r="G16" s="58" t="s">
-        <v>128</v>
       </c>
       <c r="H16" s="59"/>
       <c r="I16" s="126"/>
@@ -8397,7 +8394,7 @@
       <c r="A17" s="46"/>
       <c r="B17" s="60"/>
       <c r="C17" s="61" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D17" s="62"/>
       <c r="E17" s="63"/>
@@ -8426,41 +8423,41 @@
         <v>2</v>
       </c>
       <c r="C18" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="68" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="68" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="68" t="s">
-        <v>119</v>
-      </c>
-      <c r="E18" s="68" t="s">
-        <v>131</v>
-      </c>
       <c r="F18" s="69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G18" s="70"/>
       <c r="H18" s="71" t="s">
+        <v>131</v>
+      </c>
+      <c r="I18" s="71" t="s">
         <v>132</v>
       </c>
-      <c r="I18" s="71" t="s">
+      <c r="J18" s="128" t="s">
         <v>133</v>
       </c>
-      <c r="J18" s="128" t="s">
-        <v>134</v>
-      </c>
       <c r="K18" s="71" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L18" s="59"/>
       <c r="M18" s="59"/>
       <c r="N18" s="59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O18" s="59"/>
       <c r="P18" s="59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q18" s="59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="R18" s="154"/>
       <c r="S18" s="46"/>
@@ -8476,10 +8473,10 @@
       <c r="D19" s="73"/>
       <c r="E19" s="73"/>
       <c r="F19" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="G19" s="58" t="s">
         <v>135</v>
-      </c>
-      <c r="G19" s="58" t="s">
-        <v>136</v>
       </c>
       <c r="H19" s="71"/>
       <c r="I19" s="71"/>
@@ -8502,7 +8499,7 @@
       <c r="A20" s="46"/>
       <c r="B20" s="60"/>
       <c r="C20" s="74" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D20" s="75"/>
       <c r="E20" s="76"/>
@@ -8532,43 +8529,43 @@
         <v>3</v>
       </c>
       <c r="C21" s="80" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="81" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="81" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="81" t="s">
-        <v>119</v>
-      </c>
-      <c r="E21" s="81" t="s">
-        <v>139</v>
-      </c>
       <c r="F21" s="69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G21" s="70"/>
       <c r="H21" s="82" t="s">
+        <v>139</v>
+      </c>
+      <c r="I21" s="82" t="s">
+        <v>132</v>
+      </c>
+      <c r="J21" s="130" t="s">
         <v>140</v>
       </c>
-      <c r="I21" s="82" t="s">
-        <v>133</v>
-      </c>
-      <c r="J21" s="130" t="s">
-        <v>141</v>
-      </c>
       <c r="K21" s="82" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L21" s="131"/>
       <c r="M21" s="131"/>
       <c r="N21" s="131" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O21" s="131" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P21" s="131" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q21" s="131" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="R21" s="157"/>
       <c r="S21" s="46"/>
@@ -8584,10 +8581,10 @@
       <c r="D22" s="55"/>
       <c r="E22" s="56"/>
       <c r="F22" s="57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G22" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H22" s="59"/>
       <c r="I22" s="126"/>
@@ -8610,7 +8607,7 @@
       <c r="A23" s="46"/>
       <c r="B23" s="60"/>
       <c r="C23" s="74" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D23" s="84"/>
       <c r="E23" s="85"/>
@@ -8640,43 +8637,43 @@
         <v>4</v>
       </c>
       <c r="C24" s="80" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="81" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="81" t="s">
         <v>144</v>
       </c>
-      <c r="D24" s="81" t="s">
-        <v>119</v>
-      </c>
-      <c r="E24" s="81" t="s">
-        <v>145</v>
-      </c>
       <c r="F24" s="69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G24" s="70"/>
       <c r="H24" s="82" t="s">
+        <v>145</v>
+      </c>
+      <c r="I24" s="82" t="s">
         <v>146</v>
       </c>
-      <c r="I24" s="82" t="s">
+      <c r="J24" s="130" t="s">
         <v>147</v>
       </c>
-      <c r="J24" s="130" t="s">
+      <c r="K24" s="82" t="s">
         <v>148</v>
-      </c>
-      <c r="K24" s="82" t="s">
-        <v>149</v>
       </c>
       <c r="L24" s="131"/>
       <c r="M24" s="131"/>
       <c r="N24" s="131" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O24" s="131" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P24" s="131" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q24" s="131" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="R24" s="157"/>
       <c r="S24" s="46"/>
@@ -8692,10 +8689,10 @@
       <c r="D25" s="55"/>
       <c r="E25" s="56"/>
       <c r="F25" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="G25" s="58" t="s">
         <v>150</v>
-      </c>
-      <c r="G25" s="58" t="s">
-        <v>151</v>
       </c>
       <c r="H25" s="59"/>
       <c r="I25" s="126"/>
@@ -8718,7 +8715,7 @@
       <c r="A26" s="46"/>
       <c r="B26" s="86"/>
       <c r="C26" s="87" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D26" s="62"/>
       <c r="E26" s="63"/>
@@ -8748,34 +8745,34 @@
         <v>5</v>
       </c>
       <c r="C27" s="90" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" s="91" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="91" t="s">
         <v>153</v>
       </c>
-      <c r="D27" s="91" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" s="91" t="s">
-        <v>154</v>
-      </c>
       <c r="F27" s="92" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G27" s="93"/>
       <c r="H27" s="94" t="s">
+        <v>154</v>
+      </c>
+      <c r="I27" s="133" t="s">
         <v>155</v>
       </c>
-      <c r="I27" s="133" t="s">
+      <c r="J27" s="134" t="s">
+        <v>147</v>
+      </c>
+      <c r="K27" s="94" t="s">
         <v>156</v>
-      </c>
-      <c r="J27" s="134" t="s">
-        <v>148</v>
-      </c>
-      <c r="K27" s="94" t="s">
-        <v>157</v>
       </c>
       <c r="L27" s="135"/>
       <c r="M27" s="135"/>
       <c r="N27" s="135" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O27" s="135"/>
       <c r="P27" s="135"/>
@@ -8794,10 +8791,10 @@
       <c r="D28" s="55"/>
       <c r="E28" s="56"/>
       <c r="F28" s="57" t="s">
+        <v>157</v>
+      </c>
+      <c r="G28" s="58" t="s">
         <v>158</v>
-      </c>
-      <c r="G28" s="58" t="s">
-        <v>159</v>
       </c>
       <c r="H28" s="59"/>
       <c r="I28" s="59"/>
@@ -8820,7 +8817,7 @@
       <c r="A29" s="46"/>
       <c r="B29" s="96"/>
       <c r="C29" s="74" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D29" s="84"/>
       <c r="E29" s="85"/>
@@ -8850,35 +8847,35 @@
         <v>6</v>
       </c>
       <c r="C30" s="80" t="s">
+        <v>159</v>
+      </c>
+      <c r="D30" s="81" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="81" t="s">
         <v>160</v>
       </c>
-      <c r="D30" s="81" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="81" t="s">
+      <c r="F30" s="69" t="s">
         <v>161</v>
-      </c>
-      <c r="F30" s="69" t="s">
-        <v>162</v>
       </c>
       <c r="G30" s="70"/>
       <c r="H30" s="82" t="s">
+        <v>154</v>
+      </c>
+      <c r="I30" s="136" t="s">
         <v>155</v>
       </c>
-      <c r="I30" s="136" t="s">
-        <v>156</v>
-      </c>
       <c r="J30" s="130" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K30" s="82" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L30" s="131"/>
       <c r="M30" s="131"/>
       <c r="N30" s="131"/>
       <c r="O30" s="81" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P30" s="131"/>
       <c r="Q30" s="131"/>
@@ -8896,10 +8893,10 @@
       <c r="D31" s="55"/>
       <c r="E31" s="56"/>
       <c r="F31" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="G31" s="58" t="s">
         <v>164</v>
-      </c>
-      <c r="G31" s="58" t="s">
-        <v>165</v>
       </c>
       <c r="H31" s="59"/>
       <c r="I31" s="59"/>
@@ -8922,7 +8919,7 @@
       <c r="A32" s="46"/>
       <c r="B32" s="96"/>
       <c r="C32" s="74" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D32" s="84"/>
       <c r="E32" s="85"/>
@@ -8952,35 +8949,35 @@
         <v>7</v>
       </c>
       <c r="C33" s="80" t="s">
+        <v>165</v>
+      </c>
+      <c r="D33" s="81" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="81" t="s">
         <v>166</v>
       </c>
-      <c r="D33" s="81" t="s">
-        <v>119</v>
-      </c>
-      <c r="E33" s="81" t="s">
+      <c r="F33" s="69" t="s">
         <v>167</v>
-      </c>
-      <c r="F33" s="69" t="s">
-        <v>168</v>
       </c>
       <c r="G33" s="98"/>
       <c r="H33" s="82" t="s">
+        <v>168</v>
+      </c>
+      <c r="I33" s="136" t="s">
+        <v>155</v>
+      </c>
+      <c r="J33" s="130" t="s">
+        <v>147</v>
+      </c>
+      <c r="K33" s="82" t="s">
         <v>169</v>
-      </c>
-      <c r="I33" s="136" t="s">
-        <v>156</v>
-      </c>
-      <c r="J33" s="130" t="s">
-        <v>148</v>
-      </c>
-      <c r="K33" s="82" t="s">
-        <v>170</v>
       </c>
       <c r="L33" s="131"/>
       <c r="M33" s="131"/>
       <c r="N33" s="131"/>
       <c r="O33" s="81" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P33" s="131"/>
       <c r="Q33" s="131"/>
@@ -8998,10 +8995,10 @@
       <c r="D34" s="55"/>
       <c r="E34" s="56"/>
       <c r="F34" s="57" t="s">
+        <v>170</v>
+      </c>
+      <c r="G34" s="58" t="s">
         <v>171</v>
-      </c>
-      <c r="G34" s="58" t="s">
-        <v>172</v>
       </c>
       <c r="H34" s="59"/>
       <c r="I34" s="59"/>
@@ -9024,7 +9021,7 @@
       <c r="A35" s="46"/>
       <c r="B35" s="95"/>
       <c r="C35" s="99" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D35" s="100"/>
       <c r="E35" s="101"/>
@@ -9057,36 +9054,36 @@
         <v>43475</v>
       </c>
       <c r="D36" s="91" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E36" s="91" t="s">
+        <v>172</v>
+      </c>
+      <c r="F36" s="92" t="s">
         <v>173</v>
-      </c>
-      <c r="F36" s="92" t="s">
-        <v>174</v>
       </c>
       <c r="G36" s="104"/>
       <c r="H36" s="94" t="s">
+        <v>154</v>
+      </c>
+      <c r="I36" s="133" t="s">
         <v>155</v>
       </c>
-      <c r="I36" s="133" t="s">
+      <c r="J36" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="K36" s="94" t="s">
         <v>156</v>
-      </c>
-      <c r="J36" s="94" t="s">
-        <v>175</v>
-      </c>
-      <c r="K36" s="94" t="s">
-        <v>157</v>
       </c>
       <c r="L36" s="135"/>
       <c r="M36" s="91" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N36" s="91" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O36" s="91" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P36" s="135"/>
       <c r="Q36" s="135"/>
@@ -9094,7 +9091,7 @@
       <c r="S36" s="46"/>
       <c r="T36" s="153"/>
       <c r="U36" s="162" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="V36" s="153"/>
       <c r="W36" s="153"/>
@@ -9106,10 +9103,10 @@
       <c r="D37" s="73"/>
       <c r="E37" s="73"/>
       <c r="F37" s="57" t="s">
+        <v>175</v>
+      </c>
+      <c r="G37" s="58" t="s">
         <v>176</v>
-      </c>
-      <c r="G37" s="58" t="s">
-        <v>177</v>
       </c>
       <c r="H37" s="71"/>
       <c r="I37" s="137"/>
@@ -9132,7 +9129,7 @@
       <c r="A38" s="46"/>
       <c r="B38" s="105"/>
       <c r="C38" s="106" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D38" s="107"/>
       <c r="E38" s="108"/>
@@ -9340,18 +9337,18 @@
   </mergeCells>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="D4:F4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="「お持ちの資格」 or 「無し」" prompt="をご記載ください。&#10;&#10;ない場合は「無し」とご記載ください。" sqref="D7:F7"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L15:R38">
+      <formula1>"●"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="I4:R4">
       <formula1>"男性,女性,　　　　"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="いつから稼働可能か" prompt="をご記載ください。&#10;&#10;(例)「即日～」&#10;&#10;　  「○月△日～」" sqref="D6:F6"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="「路線名　駅名」" prompt="をご記載ください。&#10;&#10;(例)○○線 △△駅" sqref="D5:F5"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L15:R38">
-      <formula1>"●"</formula1>
-    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="「お持ちの資格」 or 「無し」" prompt="をご記載ください。&#10;&#10;ない場合は「無し」とご記載ください。" sqref="D7:F7"/>
   </dataValidations>
   <pageMargins left="0.236220472440945" right="0.236220472440945" top="0.984251968503937" bottom="0.984251968503937" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="portrait"/>
   <headerFooter/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="26" max="17" man="1"/>

</xml_diff>